<commit_message>
write first chunk of driving seg material
</commit_message>
<xml_diff>
--- a/support/urban_rural_classifications_by_region.xlsx
+++ b/support/urban_rural_classifications_by_region.xlsx
@@ -157,9 +157,6 @@
     <t>very remote small town 3 to 10k</t>
   </si>
   <si>
-    <t>accessibel rural - less than 3k</t>
-  </si>
-  <si>
     <t>remote rural - settlement &lt; 3k</t>
   </si>
   <si>
@@ -239,6 +236,9 @@
   </si>
   <si>
     <t>RURAL</t>
+  </si>
+  <si>
+    <t>accessible rural - less than 3k</t>
   </si>
 </sst>
 </file>
@@ -16626,7 +16626,7 @@
     </i>
   </colItems>
   <pageFields count="1">
-    <pageField fld="0" item="17" hier="-1"/>
+    <pageField fld="0" item="11" hier="-1"/>
   </pageFields>
   <dataFields count="1">
     <dataField name="Sum of Freq" fld="3" baseField="1" baseItem="0" numFmtId="10">
@@ -16955,16 +16955,17 @@
   <dimension ref="A1:O43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.5546875" customWidth="1"/>
-    <col min="3" max="3" width="6" customWidth="1"/>
+    <col min="3" max="3" width="7" customWidth="1"/>
     <col min="4" max="5" width="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="7" customWidth="1"/>
+    <col min="6" max="6" width="6" customWidth="1"/>
+    <col min="7" max="7" width="7" customWidth="1"/>
     <col min="8" max="8" width="6" customWidth="1"/>
     <col min="9" max="9" width="6" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.77734375" bestFit="1" customWidth="1"/>
@@ -16980,7 +16981,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
@@ -17040,34 +17041,34 @@
         <v>1</v>
       </c>
       <c r="B5" s="3">
-        <v>0</v>
+        <v>0.47645951035781542</v>
       </c>
       <c r="C5" s="3">
-        <v>0</v>
+        <v>0.31450094161958569</v>
       </c>
       <c r="D5" s="3">
         <v>0</v>
       </c>
       <c r="E5" s="3">
-        <v>0</v>
+        <v>4.519774011299435E-2</v>
       </c>
       <c r="F5" s="3">
-        <v>0.90731707317073174</v>
+        <v>0</v>
       </c>
       <c r="G5" s="3">
-        <v>8.7804878048780483E-2</v>
+        <v>9.9811676082862524E-2</v>
       </c>
       <c r="H5" s="3">
-        <v>4.8780487804878049E-3</v>
+        <v>6.2146892655367235E-2</v>
       </c>
       <c r="I5" s="3">
-        <v>0</v>
+        <v>1.8832391713747645E-3</v>
       </c>
       <c r="J5" s="3">
         <v>1</v>
       </c>
       <c r="K5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L5" s="4">
         <v>1</v>
@@ -17084,34 +17085,34 @@
         <v>2</v>
       </c>
       <c r="B6" s="3">
-        <v>0</v>
+        <v>0.45400000000000001</v>
       </c>
       <c r="C6" s="3">
-        <v>0</v>
+        <v>0.314</v>
       </c>
       <c r="D6" s="3">
-        <v>0</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="E6" s="3">
-        <v>0</v>
+        <v>4.3999999999999997E-2</v>
       </c>
       <c r="F6" s="3">
-        <v>0.89119170984455953</v>
+        <v>2E-3</v>
       </c>
       <c r="G6" s="3">
-        <v>8.8082901554404139E-2</v>
+        <v>0.112</v>
       </c>
       <c r="H6" s="3">
-        <v>2.072538860103627E-2</v>
+        <v>6.6000000000000003E-2</v>
       </c>
       <c r="I6" s="3">
-        <v>0</v>
+        <v>2E-3</v>
       </c>
       <c r="J6" s="3">
         <v>1</v>
       </c>
       <c r="K6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L6" s="4">
         <v>2</v>
@@ -17128,34 +17129,34 @@
         <v>3</v>
       </c>
       <c r="B7" s="3">
-        <v>0</v>
+        <v>0.46987951807228917</v>
       </c>
       <c r="C7" s="3">
-        <v>0</v>
+        <v>0.31526104417670681</v>
       </c>
       <c r="D7" s="3">
-        <v>0</v>
+        <v>1.0040160642570281E-2</v>
       </c>
       <c r="E7" s="3">
-        <v>0</v>
+        <v>4.0160642570281124E-2</v>
       </c>
       <c r="F7" s="3">
-        <v>0.87165775401069523</v>
+        <v>2.008032128514056E-3</v>
       </c>
       <c r="G7" s="3">
-        <v>0.11229946524064172</v>
+        <v>9.8393574297188757E-2</v>
       </c>
       <c r="H7" s="3">
-        <v>1.6042780748663103E-2</v>
+        <v>6.224899598393574E-2</v>
       </c>
       <c r="I7" s="3">
-        <v>0</v>
+        <v>2.008032128514056E-3</v>
       </c>
       <c r="J7" s="3">
         <v>1</v>
       </c>
       <c r="K7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L7" s="4">
         <v>3</v>
@@ -17172,34 +17173,34 @@
         <v>4</v>
       </c>
       <c r="B8" s="3">
-        <v>0</v>
+        <v>0.45194274028629855</v>
       </c>
       <c r="C8" s="3">
-        <v>0</v>
+        <v>0.33742331288343558</v>
       </c>
       <c r="D8" s="3">
-        <v>0</v>
+        <v>1.2269938650306749E-2</v>
       </c>
       <c r="E8" s="3">
-        <v>0</v>
+        <v>4.0899795501022497E-2</v>
       </c>
       <c r="F8" s="3">
-        <v>0.88235294117647056</v>
+        <v>2.0449897750511249E-3</v>
       </c>
       <c r="G8" s="3">
-        <v>0.10160427807486631</v>
+        <v>9.4069529652351741E-2</v>
       </c>
       <c r="H8" s="3">
-        <v>1.06951871657754E-2</v>
+        <v>5.9304703476482618E-2</v>
       </c>
       <c r="I8" s="3">
-        <v>5.3475935828877002E-3</v>
+        <v>2.0449897750511249E-3</v>
       </c>
       <c r="J8" s="3">
         <v>1</v>
       </c>
       <c r="K8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L8" s="4">
         <v>4</v>
@@ -17216,34 +17217,34 @@
         <v>5</v>
       </c>
       <c r="B9" s="3">
-        <v>0</v>
+        <v>0.45031712473572938</v>
       </c>
       <c r="C9" s="3">
-        <v>0</v>
+        <v>0.33615221987315008</v>
       </c>
       <c r="D9" s="3">
-        <v>0</v>
+        <v>1.2684989429175475E-2</v>
       </c>
       <c r="E9" s="3">
-        <v>0</v>
+        <v>3.8054968287526428E-2</v>
       </c>
       <c r="F9" s="3">
-        <v>0.88304093567251463</v>
+        <v>0</v>
       </c>
       <c r="G9" s="3">
-        <v>0.1111111111111111</v>
+        <v>9.7251585623678652E-2</v>
       </c>
       <c r="H9" s="3">
-        <v>5.8479532163742687E-3</v>
+        <v>6.13107822410148E-2</v>
       </c>
       <c r="I9" s="3">
-        <v>0</v>
+        <v>4.2283298097251587E-3</v>
       </c>
       <c r="J9" s="3">
         <v>1</v>
       </c>
       <c r="K9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L9" s="4">
         <v>5</v>
@@ -17260,34 +17261,34 @@
         <v>6</v>
       </c>
       <c r="B10" s="3">
-        <v>0</v>
+        <v>0.44026548672566373</v>
       </c>
       <c r="C10" s="3">
-        <v>0</v>
+        <v>0.34955752212389379</v>
       </c>
       <c r="D10" s="3">
-        <v>0</v>
+        <v>1.9911504424778761E-2</v>
       </c>
       <c r="E10" s="3">
-        <v>0</v>
+        <v>2.6548672566371681E-2</v>
       </c>
       <c r="F10" s="3">
-        <v>0.88304093567251463</v>
+        <v>0</v>
       </c>
       <c r="G10" s="3">
-        <v>9.9415204678362568E-2</v>
+        <v>0.10398230088495575</v>
       </c>
       <c r="H10" s="3">
-        <v>1.1695906432748537E-2</v>
+        <v>5.7522123893805309E-2</v>
       </c>
       <c r="I10" s="3">
-        <v>5.8479532163742687E-3</v>
+        <v>2.2123893805309734E-3</v>
       </c>
       <c r="J10" s="3">
         <v>1</v>
       </c>
       <c r="K10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="L10" s="4">
         <v>6</v>
@@ -17296,7 +17297,7 @@
         <v>30</v>
       </c>
       <c r="O10" t="s">
-        <v>43</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
@@ -17304,34 +17305,34 @@
         <v>7</v>
       </c>
       <c r="B11" s="3">
-        <v>0</v>
+        <v>0.40211640211640209</v>
       </c>
       <c r="C11" s="3">
-        <v>0</v>
+        <v>0.36684303350970016</v>
       </c>
       <c r="D11" s="3">
-        <v>0</v>
+        <v>5.4673721340388004E-2</v>
       </c>
       <c r="E11" s="3">
-        <v>0</v>
+        <v>1.9400352733686066E-2</v>
       </c>
       <c r="F11" s="3">
-        <v>0.8878048780487805</v>
+        <v>0</v>
       </c>
       <c r="G11" s="3">
-        <v>9.2682926829268292E-2</v>
+        <v>0.10582010582010581</v>
       </c>
       <c r="H11" s="3">
-        <v>1.4634146341463415E-2</v>
+        <v>4.9382716049382713E-2</v>
       </c>
       <c r="I11" s="3">
-        <v>4.8780487804878049E-3</v>
+        <v>1.7636684303350969E-3</v>
       </c>
       <c r="J11" s="3">
         <v>1</v>
       </c>
       <c r="K11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="L11" s="4">
         <v>7</v>
@@ -17340,7 +17341,7 @@
         <v>32</v>
       </c>
       <c r="O11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
@@ -17348,34 +17349,34 @@
         <v>8</v>
       </c>
       <c r="B12" s="3">
-        <v>0</v>
+        <v>0.3830570902394107</v>
       </c>
       <c r="C12" s="3">
-        <v>0</v>
+        <v>0.36648250460405157</v>
       </c>
       <c r="D12" s="3">
-        <v>0</v>
+        <v>6.0773480662983423E-2</v>
       </c>
       <c r="E12" s="3">
-        <v>0</v>
+        <v>2.5782688766114181E-2</v>
       </c>
       <c r="F12" s="3">
-        <v>0.89473684210526316</v>
+        <v>0</v>
       </c>
       <c r="G12" s="3">
-        <v>9.0909090909090912E-2</v>
+        <v>0.11049723756906077</v>
       </c>
       <c r="H12" s="3">
-        <v>9.5693779904306216E-3</v>
+        <v>5.1565377532228361E-2</v>
       </c>
       <c r="I12" s="3">
-        <v>4.7846889952153108E-3</v>
+        <v>1.841620626151013E-3</v>
       </c>
       <c r="J12" s="3">
         <v>1</v>
       </c>
       <c r="K12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="L12" s="4">
         <v>8</v>
@@ -17384,7 +17385,7 @@
         <v>34</v>
       </c>
       <c r="O12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
@@ -17392,28 +17393,28 @@
         <v>9</v>
       </c>
       <c r="B13" s="3">
-        <v>0</v>
+        <v>0.40918163672654689</v>
       </c>
       <c r="C13" s="3">
-        <v>0</v>
+        <v>0.29241516966067865</v>
       </c>
       <c r="D13" s="3">
-        <v>0</v>
+        <v>8.4331337325349295E-2</v>
       </c>
       <c r="E13" s="3">
-        <v>0</v>
+        <v>1.7964071856287425E-2</v>
       </c>
       <c r="F13" s="3">
-        <v>0.88059701492537312</v>
+        <v>5.4890219560878245E-3</v>
       </c>
       <c r="G13" s="3">
-        <v>8.9552238805970144E-2</v>
+        <v>0.14021956087824353</v>
       </c>
       <c r="H13" s="3">
-        <v>1.4925373134328358E-2</v>
+        <v>2.5948103792415168E-2</v>
       </c>
       <c r="I13" s="3">
-        <v>1.4925373134328358E-2</v>
+        <v>2.4451097804391218E-2</v>
       </c>
       <c r="J13" s="3">
         <v>1</v>
@@ -17425,28 +17426,28 @@
         <v>10</v>
       </c>
       <c r="B14" s="3">
-        <v>0</v>
+        <v>0.39243614931237719</v>
       </c>
       <c r="C14" s="3">
-        <v>0</v>
+        <v>0.30009823182711198</v>
       </c>
       <c r="D14" s="3">
-        <v>0</v>
+        <v>9.4793713163064827E-2</v>
       </c>
       <c r="E14" s="3">
-        <v>0</v>
+        <v>1.8664047151277015E-2</v>
       </c>
       <c r="F14" s="3">
-        <v>0.88725490196078427</v>
+        <v>6.8762278978389E-3</v>
       </c>
       <c r="G14" s="3">
-        <v>8.8235294117647065E-2</v>
+        <v>0.14047151277013753</v>
       </c>
       <c r="H14" s="3">
-        <v>4.9019607843137254E-3</v>
+        <v>2.6522593320235755E-2</v>
       </c>
       <c r="I14" s="3">
-        <v>1.9607843137254902E-2</v>
+        <v>2.0137524557956778E-2</v>
       </c>
       <c r="J14" s="3">
         <v>1</v>
@@ -17457,28 +17458,28 @@
         <v>11</v>
       </c>
       <c r="B15" s="3">
-        <v>0</v>
+        <v>0.38961693548387094</v>
       </c>
       <c r="C15" s="3">
-        <v>0</v>
+        <v>0.30544354838709675</v>
       </c>
       <c r="D15" s="3">
-        <v>0</v>
+        <v>9.6270161290322578E-2</v>
       </c>
       <c r="E15" s="3">
-        <v>0</v>
+        <v>1.8145161290322582E-2</v>
       </c>
       <c r="F15" s="3">
-        <v>0.89162561576354682</v>
+        <v>7.5604838709677422E-3</v>
       </c>
       <c r="G15" s="3">
-        <v>7.8817733990147784E-2</v>
+        <v>0.13760080645161291</v>
       </c>
       <c r="H15" s="3">
-        <v>1.4778325123152709E-2</v>
+        <v>2.5201612903225805E-2</v>
       </c>
       <c r="I15" s="3">
-        <v>1.4778325123152709E-2</v>
+        <v>2.0161290322580645E-2</v>
       </c>
       <c r="J15" s="3">
         <v>1</v>
@@ -17489,28 +17490,28 @@
         <v>12</v>
       </c>
       <c r="B16" s="3">
-        <v>0</v>
+        <v>0.3888888888888889</v>
       </c>
       <c r="C16" s="3">
-        <v>0</v>
+        <v>0.29966329966329969</v>
       </c>
       <c r="D16" s="3">
-        <v>0</v>
+        <v>9.1470258136924804E-2</v>
       </c>
       <c r="E16" s="3">
-        <v>0</v>
+        <v>1.9079685746352413E-2</v>
       </c>
       <c r="F16" s="3">
-        <v>0.90123456790123457</v>
+        <v>8.9786756453423128E-3</v>
       </c>
       <c r="G16" s="3">
-        <v>8.0246913580246909E-2</v>
+        <v>0.14141414141414141</v>
       </c>
       <c r="H16" s="3">
-        <v>1.2345679012345678E-2</v>
+        <v>2.8619528619528621E-2</v>
       </c>
       <c r="I16" s="3">
-        <v>6.1728395061728392E-3</v>
+        <v>2.1885521885521887E-2</v>
       </c>
       <c r="J16" s="3">
         <v>1</v>
@@ -17521,28 +17522,28 @@
         <v>13</v>
       </c>
       <c r="B17" s="3">
-        <v>0</v>
+        <v>0.39216832261835183</v>
       </c>
       <c r="C17" s="3">
-        <v>0</v>
+        <v>0.29748684979544127</v>
       </c>
       <c r="D17" s="3">
-        <v>0</v>
+        <v>9.409701928696669E-2</v>
       </c>
       <c r="E17" s="3">
-        <v>0</v>
+        <v>2.1040327293980129E-2</v>
       </c>
       <c r="F17" s="3">
-        <v>0.89171974522292996</v>
+        <v>8.1823495032144946E-3</v>
       </c>
       <c r="G17" s="3">
-        <v>7.6433121019108277E-2</v>
+        <v>0.13559322033898305</v>
       </c>
       <c r="H17" s="3">
-        <v>1.2738853503184714E-2</v>
+        <v>2.863822326125073E-2</v>
       </c>
       <c r="I17" s="3">
-        <v>1.9108280254777069E-2</v>
+        <v>2.2793687901811806E-2</v>
       </c>
       <c r="J17" s="3">
         <v>1</v>
@@ -17553,28 +17554,28 @@
         <v>14</v>
       </c>
       <c r="B18" s="3">
-        <v>0</v>
+        <v>0.38387484957882068</v>
       </c>
       <c r="C18" s="3">
-        <v>0</v>
+        <v>0.29542719614921781</v>
       </c>
       <c r="D18" s="3">
-        <v>0</v>
+        <v>9.5667870036101083E-2</v>
       </c>
       <c r="E18" s="3">
-        <v>0</v>
+        <v>2.3465703971119134E-2</v>
       </c>
       <c r="F18" s="3">
-        <v>0.89542483660130723</v>
+        <v>8.4235860409145602E-3</v>
       </c>
       <c r="G18" s="3">
-        <v>7.8431372549019607E-2</v>
+        <v>0.14139590854392298</v>
       </c>
       <c r="H18" s="3">
-        <v>1.3071895424836602E-2</v>
+        <v>2.9482551143200964E-2</v>
       </c>
       <c r="I18" s="3">
-        <v>1.3071895424836602E-2</v>
+        <v>2.2262334536702767E-2</v>
       </c>
       <c r="J18" s="3">
         <v>1</v>
@@ -17585,28 +17586,28 @@
         <v>15</v>
       </c>
       <c r="B19" s="3">
-        <v>0</v>
+        <v>0.37928921568627449</v>
       </c>
       <c r="C19" s="3">
-        <v>0</v>
+        <v>0.29105392156862747</v>
       </c>
       <c r="D19" s="3">
-        <v>0</v>
+        <v>8.8235294117647065E-2</v>
       </c>
       <c r="E19" s="3">
-        <v>0</v>
+        <v>2.7573529411764705E-2</v>
       </c>
       <c r="F19" s="3">
-        <v>0.87341772151898733</v>
+        <v>9.1911764705882356E-3</v>
       </c>
       <c r="G19" s="3">
-        <v>9.49367088607595E-2</v>
+        <v>0.1482843137254902</v>
       </c>
       <c r="H19" s="3">
-        <v>1.8987341772151899E-2</v>
+        <v>3.2475490196078434E-2</v>
       </c>
       <c r="I19" s="3">
-        <v>1.2658227848101266E-2</v>
+        <v>2.389705882352941E-2</v>
       </c>
       <c r="J19" s="3">
         <v>1</v>
@@ -17617,28 +17618,28 @@
         <v>16</v>
       </c>
       <c r="B20" s="3">
-        <v>0</v>
+        <v>0.38721804511278196</v>
       </c>
       <c r="C20" s="3">
-        <v>0</v>
+        <v>0.29010025062656641</v>
       </c>
       <c r="D20" s="3">
-        <v>0</v>
+        <v>8.834586466165413E-2</v>
       </c>
       <c r="E20" s="3">
-        <v>0</v>
+        <v>2.3809523809523808E-2</v>
       </c>
       <c r="F20" s="3">
-        <v>0.87116564417177911</v>
+        <v>9.3984962406015032E-3</v>
       </c>
       <c r="G20" s="3">
-        <v>8.5889570552147243E-2</v>
+        <v>0.14598997493734336</v>
       </c>
       <c r="H20" s="3">
-        <v>3.0674846625766871E-2</v>
+        <v>3.007518796992481E-2</v>
       </c>
       <c r="I20" s="3">
-        <v>1.2269938650306749E-2</v>
+        <v>2.5062656641604009E-2</v>
       </c>
       <c r="J20" s="3">
         <v>1</v>
@@ -17649,28 +17650,28 @@
         <v>17</v>
       </c>
       <c r="B21" s="3">
-        <v>0</v>
+        <v>0.37681159420289856</v>
       </c>
       <c r="C21" s="3">
-        <v>0</v>
+        <v>0.29710144927536231</v>
       </c>
       <c r="D21" s="3">
-        <v>0</v>
+        <v>8.8932806324110672E-2</v>
       </c>
       <c r="E21" s="3">
-        <v>0</v>
+        <v>2.5691699604743084E-2</v>
       </c>
       <c r="F21" s="3">
-        <v>0.86538461538461542</v>
+        <v>8.563899868247694E-3</v>
       </c>
       <c r="G21" s="3">
-        <v>8.9743589743589744E-2</v>
+        <v>0.14426877470355731</v>
       </c>
       <c r="H21" s="3">
-        <v>3.2051282051282048E-2</v>
+        <v>3.2279314888010543E-2</v>
       </c>
       <c r="I21" s="3">
-        <v>1.282051282051282E-2</v>
+        <v>2.6350461133069828E-2</v>
       </c>
       <c r="J21" s="3">
         <v>1</v>
@@ -17681,28 +17682,28 @@
         <v>18</v>
       </c>
       <c r="B22" s="3">
-        <v>0</v>
+        <v>0.37742150968603877</v>
       </c>
       <c r="C22" s="3">
-        <v>0</v>
+        <v>0.29124916499665998</v>
       </c>
       <c r="D22" s="3">
-        <v>0</v>
+        <v>9.2852371409485643E-2</v>
       </c>
       <c r="E22" s="3">
-        <v>0</v>
+        <v>2.8056112224448898E-2</v>
       </c>
       <c r="F22" s="3">
-        <v>0.86538461538461542</v>
+        <v>8.6840347361389451E-3</v>
       </c>
       <c r="G22" s="3">
-        <v>9.6153846153846159E-2</v>
+        <v>0.14696058784235136</v>
       </c>
       <c r="H22" s="3">
-        <v>2.564102564102564E-2</v>
+        <v>3.0060120240480961E-2</v>
       </c>
       <c r="I22" s="3">
-        <v>1.282051282051282E-2</v>
+        <v>2.4716098864395457E-2</v>
       </c>
       <c r="J22" s="3">
         <v>1</v>
@@ -17713,28 +17714,28 @@
         <v>23</v>
       </c>
       <c r="B23" s="3">
-        <v>0</v>
+        <v>0.3981839348079162</v>
       </c>
       <c r="C23" s="3">
-        <v>0</v>
+        <v>0.30416763678696157</v>
       </c>
       <c r="D23" s="3">
-        <v>0</v>
+        <v>7.8603026775320134E-2</v>
       </c>
       <c r="E23" s="3">
-        <v>0</v>
+        <v>2.4400465657741559E-2</v>
       </c>
       <c r="F23" s="3">
-        <v>0.88522061092255477</v>
+        <v>6.6589057043073344E-3</v>
       </c>
       <c r="G23" s="3">
-        <v>9.1329836470225245E-2</v>
+        <v>0.13457508731082654</v>
       </c>
       <c r="H23" s="3">
-        <v>1.4810243751928418E-2</v>
+        <v>3.4318975552968568E-2</v>
       </c>
       <c r="I23" s="3">
-        <v>8.6393088552915772E-3</v>
+        <v>1.9091967403958091E-2</v>
       </c>
       <c r="J23" s="3">
         <v>1</v>
@@ -17742,19 +17743,19 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C25" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K25" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="L25" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="L25" s="5" t="s">
+      <c r="M25" s="5" t="s">
         <v>50</v>
-      </c>
-      <c r="M25" s="5" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
@@ -17765,7 +17766,7 @@
         <v>1991</v>
       </c>
       <c r="K26" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L26" s="10">
         <v>0.53901411939559074</v>
@@ -17783,7 +17784,7 @@
         <v>1992</v>
       </c>
       <c r="K27" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L27" s="10">
         <v>0.6009825327510917</v>
@@ -17801,7 +17802,7 @@
         <v>1993</v>
       </c>
       <c r="K28" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L28" s="10">
         <v>0.60565167243367934</v>
@@ -17819,7 +17820,7 @@
         <v>1994</v>
       </c>
       <c r="K29" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L29" s="10">
         <v>0.66302952503209245</v>
@@ -17837,7 +17838,7 @@
         <v>1995</v>
       </c>
       <c r="K30" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L30" s="10">
         <v>0.67039641943734019</v>
@@ -17855,7 +17856,7 @@
         <v>1996</v>
       </c>
       <c r="K31" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L31" s="10">
         <v>0.72105324343176003</v>
@@ -17873,7 +17874,7 @@
         <v>1997</v>
       </c>
       <c r="K32" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L32" s="10">
         <v>0.75247733502002956</v>
@@ -17891,10 +17892,10 @@
         <v>1998</v>
       </c>
       <c r="E33" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K33" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L33" s="10">
         <v>0.78712190650779101</v>
@@ -17912,7 +17913,7 @@
         <v>1999</v>
       </c>
       <c r="K34" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L34" s="10">
         <v>0.88522061092255477</v>
@@ -17930,7 +17931,7 @@
         <v>2000</v>
       </c>
       <c r="K35" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L35" s="10">
         <v>0.95353377586880128</v>
@@ -17948,7 +17949,7 @@
         <v>2001</v>
       </c>
       <c r="K36" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L36" s="10">
         <v>0.96926503340757242</v>
@@ -17966,7 +17967,7 @@
         <v>2002</v>
       </c>
       <c r="K37" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L37" s="10">
         <v>0.96953316953316948</v>
@@ -17984,7 +17985,7 @@
         <v>2003</v>
       </c>
       <c r="K38" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L38" s="10">
         <v>0.98971797884841362</v>
@@ -18002,7 +18003,7 @@
         <v>2004</v>
       </c>
       <c r="K39" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L39" s="10">
         <v>0.99115274525110586</v>
@@ -18020,7 +18021,7 @@
         <v>2005</v>
       </c>
       <c r="K40" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L40" s="10">
         <v>0.99547511312217196</v>
@@ -18038,7 +18039,7 @@
         <v>2006</v>
       </c>
       <c r="K41" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L41" s="10">
         <v>1</v>
@@ -18100,8 +18101,88 @@
           <x14:colorLow rgb="FFD00000"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>Sheet1!B5:B22</xm:f>
-              <xm:sqref>M5</xm:sqref>
+              <xm:f>Sheet1!I5:I22</xm:f>
+              <xm:sqref>M12</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup displayEmptyCellsAs="gap">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>Sheet1!H5:H22</xm:f>
+              <xm:sqref>M11</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup displayEmptyCellsAs="gap">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>Sheet1!G5:G22</xm:f>
+              <xm:sqref>M10</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup displayEmptyCellsAs="gap">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>Sheet1!F5:F22</xm:f>
+              <xm:sqref>M9</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup displayEmptyCellsAs="gap">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>Sheet1!E5:E22</xm:f>
+              <xm:sqref>M8</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup displayEmptyCellsAs="gap">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>Sheet1!D5:D22</xm:f>
+              <xm:sqref>M7</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
@@ -18132,88 +18213,8 @@
           <x14:colorLow rgb="FFD00000"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>Sheet1!D5:D22</xm:f>
-              <xm:sqref>M7</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="gap">
-          <x14:colorSeries rgb="FF376092"/>
-          <x14:colorNegative rgb="FFD00000"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FFD00000"/>
-          <x14:colorFirst rgb="FFD00000"/>
-          <x14:colorLast rgb="FFD00000"/>
-          <x14:colorHigh rgb="FFD00000"/>
-          <x14:colorLow rgb="FFD00000"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>Sheet1!E5:E22</xm:f>
-              <xm:sqref>M8</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="gap">
-          <x14:colorSeries rgb="FF376092"/>
-          <x14:colorNegative rgb="FFD00000"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FFD00000"/>
-          <x14:colorFirst rgb="FFD00000"/>
-          <x14:colorLast rgb="FFD00000"/>
-          <x14:colorHigh rgb="FFD00000"/>
-          <x14:colorLow rgb="FFD00000"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>Sheet1!F5:F22</xm:f>
-              <xm:sqref>M9</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="gap">
-          <x14:colorSeries rgb="FF376092"/>
-          <x14:colorNegative rgb="FFD00000"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FFD00000"/>
-          <x14:colorFirst rgb="FFD00000"/>
-          <x14:colorLast rgb="FFD00000"/>
-          <x14:colorHigh rgb="FFD00000"/>
-          <x14:colorLow rgb="FFD00000"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>Sheet1!G5:G22</xm:f>
-              <xm:sqref>M10</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="gap">
-          <x14:colorSeries rgb="FF376092"/>
-          <x14:colorNegative rgb="FFD00000"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FFD00000"/>
-          <x14:colorFirst rgb="FFD00000"/>
-          <x14:colorLast rgb="FFD00000"/>
-          <x14:colorHigh rgb="FFD00000"/>
-          <x14:colorLow rgb="FFD00000"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>Sheet1!H5:H22</xm:f>
-              <xm:sqref>M11</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="gap">
-          <x14:colorSeries rgb="FF376092"/>
-          <x14:colorNegative rgb="FFD00000"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FFD00000"/>
-          <x14:colorFirst rgb="FFD00000"/>
-          <x14:colorLast rgb="FFD00000"/>
-          <x14:colorHigh rgb="FFD00000"/>
-          <x14:colorLow rgb="FFD00000"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>Sheet1!I5:I22</xm:f>
-              <xm:sqref>M12</xm:sqref>
+              <xm:f>Sheet1!B5:B22</xm:f>
+              <xm:sqref>M5</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
@@ -18227,7 +18228,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2593"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A196" workbookViewId="0">
       <selection sqref="A1:D1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>